<commit_message>
added some dummy venue address and managing office scotland addresses
</commit_message>
<xml_diff>
--- a/src/main/resources/venueAddressValues.xlsx
+++ b/src/main/resources/venueAddressValues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rabab/HMCTS/ethos-repl-docmosis-service/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CE73E0-6079-FA46-8AB8-B92040B43CFD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07D29E4-63CC-4F4A-8405-59D7ECE2A123}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="9" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
   </bookViews>
   <sheets>
     <sheet name="Bristol" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="186">
   <si>
     <t>Leeds</t>
   </si>
@@ -584,82 +584,16 @@
     <t>Edinburgh</t>
   </si>
   <si>
-    <t>Hull Venue, Address.</t>
-  </si>
-  <si>
-    <t>IAC Venue, Address.</t>
-  </si>
-  <si>
-    <t>Leeds Venue, Address.</t>
-  </si>
-  <si>
-    <t>Scarborough Venue, Address.</t>
-  </si>
-  <si>
-    <t>Sheffield Combi Venue, Address.</t>
-  </si>
-  <si>
-    <t>Teesside ET Venue, Address.</t>
-  </si>
-  <si>
-    <t>Wakefield Count Venue, Address.</t>
-  </si>
-  <si>
-    <t>Barrow Venue, Address.</t>
-  </si>
-  <si>
-    <t>Blackpool Mags Venue, Address.</t>
-  </si>
-  <si>
-    <t>Burnley Court Venue, Address.</t>
-  </si>
-  <si>
-    <t>Carlisle C C Venue, Address.</t>
-  </si>
-  <si>
-    <t>Carlisle Mags Venue, Address.</t>
-  </si>
-  <si>
-    <t>Crown Court Venue, Address.</t>
-  </si>
-  <si>
-    <t>Fleetwood Venue, Address.</t>
-  </si>
-  <si>
-    <t>Kendal Venue, Address.</t>
-  </si>
-  <si>
-    <t>Lancaster Venue, Address.</t>
-  </si>
-  <si>
-    <t>Liverpool Venue, Address.</t>
-  </si>
-  <si>
-    <t>Manchester Venue, Address.</t>
-  </si>
-  <si>
-    <t>Manchester IA Venue, Address.</t>
-  </si>
-  <si>
-    <t>Manchester Mags Venue, Address.</t>
-  </si>
-  <si>
-    <t>Minshull Street Venue, Address.</t>
-  </si>
-  <si>
-    <t>St. Helens Venue, Address.</t>
-  </si>
-  <si>
-    <t>Glasgow Venue, Address.</t>
-  </si>
-  <si>
-    <t>Aberdeen Venue, Address.</t>
-  </si>
-  <si>
-    <t>Dundee Venue, Address.</t>
-  </si>
-  <si>
-    <t>Edinburgh Venue, Address.</t>
+    <t>54-56 Melville Street, Edinburgh, EH3 7HF</t>
+  </si>
+  <si>
+    <t>Ground Floor, Block C, Caledonian House, Greenmarket, Dundee, DD1 4QB</t>
+  </si>
+  <si>
+    <t>Ground Floor, AB1, 48 Huntly Street, Aberdeen, AB10 1SH</t>
+  </si>
+  <si>
+    <t>Eagle Building, 215 Bothwell Street, Glasgow, G2 7TS</t>
   </si>
 </sst>
 </file>
@@ -744,7 +678,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -755,11 +689,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1076,8 +1009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D604D91D-6235-9B48-BBC4-151657576CA7}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1098,194 +1031,311 @@
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1298,8 +1348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DABB460-37E4-BC4E-8C69-80DBA2CDCD9B}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1317,11 +1367,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>178</v>
       </c>
       <c r="B2" t="s">
-        <v>204</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1329,7 +1379,7 @@
         <v>179</v>
       </c>
       <c r="B3" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1337,7 +1387,7 @@
         <v>180</v>
       </c>
       <c r="B4" t="s">
-        <v>206</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1345,7 +1395,7 @@
         <v>181</v>
       </c>
       <c r="B5" t="s">
-        <v>207</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -1358,7 +1408,7 @@
   <dimension ref="A1:B66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1379,324 +1429,519 @@
       <c r="A2" s="2" t="s">
         <v>104</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>105</v>
       </c>
+      <c r="B3" s="4" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>106</v>
       </c>
+      <c r="B4" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>107</v>
       </c>
+      <c r="B5" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>108</v>
       </c>
+      <c r="B6" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>109</v>
       </c>
+      <c r="B7" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>110</v>
       </c>
+      <c r="B8" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>111</v>
       </c>
+      <c r="B9" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>112</v>
       </c>
+      <c r="B10" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>113</v>
       </c>
+      <c r="B11" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>114</v>
       </c>
+      <c r="B12" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>115</v>
       </c>
+      <c r="B13" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>116</v>
       </c>
+      <c r="B14" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>117</v>
       </c>
+      <c r="B15" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B66" s="3" t="s">
         <v>168</v>
       </c>
     </row>
@@ -1710,7 +1955,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1731,64 +1976,103 @@
       <c r="A2" s="7" t="s">
         <v>169</v>
       </c>
+      <c r="B2" s="7" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>170</v>
       </c>
+      <c r="B3" s="7" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>74</v>
       </c>
+      <c r="B4" s="7" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>171</v>
       </c>
+      <c r="B5" s="7" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>89</v>
       </c>
+      <c r="B6" s="7" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>90</v>
       </c>
+      <c r="B7" s="7" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>172</v>
       </c>
+      <c r="B8" s="7" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>51</v>
       </c>
+      <c r="B9" s="7" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>173</v>
       </c>
+      <c r="B10" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>174</v>
       </c>
+      <c r="B11" s="7" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>175</v>
       </c>
+      <c r="B12" s="7" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>176</v>
       </c>
+      <c r="B13" s="7" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>177</v>
       </c>
     </row>
@@ -1802,7 +2086,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1823,8 +2107,8 @@
       <c r="A2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B2" t="s">
-        <v>182</v>
+      <c r="B2" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1832,7 +2116,7 @@
         <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>183</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1840,7 +2124,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>184</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1848,7 +2132,7 @@
         <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>185</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1856,7 +2140,7 @@
         <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>186</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1864,15 +2148,15 @@
         <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B8" t="s">
-        <v>188</v>
+      <c r="B8" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1885,7 +2169,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1906,19 +2190,31 @@
       <c r="A2" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>50</v>
       </c>
+      <c r="B3" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>51</v>
       </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1932,7 +2228,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1953,19 +2249,31 @@
       <c r="A2" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>54</v>
       </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>55</v>
       </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1979,7 +2287,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2000,14 +2308,23 @@
       <c r="A2" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>58</v>
       </c>
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2021,7 +2338,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2042,120 +2359,120 @@
       <c r="A2" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B2" t="s">
-        <v>189</v>
+      <c r="B2" s="5" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B3" t="s">
-        <v>190</v>
+      <c r="B3" s="5" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B4" t="s">
-        <v>191</v>
+      <c r="B4" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B5" t="s">
-        <v>192</v>
+      <c r="B5" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B6" t="s">
-        <v>193</v>
+      <c r="B6" s="5" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B7" t="s">
-        <v>194</v>
+      <c r="B7" s="5" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B8" t="s">
-        <v>195</v>
+      <c r="B8" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B9" t="s">
-        <v>196</v>
+      <c r="B9" s="5" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B10" t="s">
-        <v>197</v>
+      <c r="B10" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B11" t="s">
-        <v>198</v>
+      <c r="B11" s="5" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B12" t="s">
-        <v>199</v>
+      <c r="B12" s="5" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B13" t="s">
-        <v>200</v>
+      <c r="B13" s="5" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B14" t="s">
-        <v>201</v>
+      <c r="B14" s="5" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B15" t="s">
-        <v>202</v>
+      <c r="B15" s="5" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B16" t="s">
-        <v>203</v>
+      <c r="B16" s="5" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2168,7 +2485,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2189,69 +2506,111 @@
       <c r="A2" s="6" t="s">
         <v>74</v>
       </c>
+      <c r="B2" s="6" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>75</v>
       </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>76</v>
       </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>77</v>
       </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>78</v>
       </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>79</v>
       </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>51</v>
       </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>80</v>
       </c>
+      <c r="B9" s="7" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>81</v>
       </c>
+      <c r="B10" s="7" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>82</v>
       </c>
+      <c r="B11" s="7" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>83</v>
       </c>
+      <c r="B12" s="5" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>84</v>
       </c>
+      <c r="B13" s="5" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>85</v>
       </c>
+      <c r="B14" s="5" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2265,7 +2624,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2286,44 +2645,71 @@
       <c r="A2" s="2" t="s">
         <v>87</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>88</v>
       </c>
+      <c r="B3" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>89</v>
       </c>
+      <c r="B4" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>90</v>
       </c>
+      <c r="B5" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>91</v>
       </c>
+      <c r="B6" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>78</v>
       </c>
+      <c r="B7" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>92</v>
       </c>
+      <c r="B8" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>93</v>
       </c>
+      <c r="B9" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2337,7 +2723,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2358,44 +2744,71 @@
       <c r="A2" s="2" t="s">
         <v>95</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>96</v>
       </c>
+      <c r="B3" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>97</v>
       </c>
+      <c r="B4" s="4" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>98</v>
       </c>
+      <c r="B5" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>99</v>
       </c>
+      <c r="B6" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>100</v>
       </c>
+      <c r="B7" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>101</v>
       </c>
+      <c r="B8" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>102</v>
       </c>
+      <c r="B9" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" t="s">
         <v>103</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added venue addresses for England Wales and Scotland
</commit_message>
<xml_diff>
--- a/src/main/resources/venueAddressValues.xlsx
+++ b/src/main/resources/venueAddressValues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rabab/HMCTS/ethos-repl-docmosis-service/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07D29E4-63CC-4F4A-8405-59D7ECE2A123}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03AE8524-6EF0-CD4E-8BBF-60C50600BCA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="9" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
   </bookViews>
   <sheets>
     <sheet name="Bristol" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="233">
   <si>
     <t>Leeds</t>
   </si>
@@ -587,20 +587,184 @@
     <t>54-56 Melville Street, Edinburgh, EH3 7HF</t>
   </si>
   <si>
-    <t>Ground Floor, Block C, Caledonian House, Greenmarket, Dundee, DD1 4QB</t>
-  </si>
-  <si>
     <t>Ground Floor, AB1, 48 Huntly Street, Aberdeen, AB10 1SH</t>
   </si>
   <si>
-    <t>Eagle Building, 215 Bothwell Street, Glasgow, G2 7TS</t>
+    <t>Bristol ET, Bristol Civil and Family Justice Centre, 2 Redcliff Street, Bristol, BS1 6GR</t>
+  </si>
+  <si>
+    <t>2 Floor, Keble House, Southernhay Gardens, Exeter, EX1 1NT</t>
+  </si>
+  <si>
+    <t>Plymouth Magistrates’ Court, St Andrews Street, Plymouth, PL1 2DP</t>
+  </si>
+  <si>
+    <t>Bodmin Magistrates’ Court, Launceston Road, Bodmin, PL31 2AL</t>
+  </si>
+  <si>
+    <t>West Hampshire Magistrates’ Court, 100 The Avenue, Southampton, SO17 1EY</t>
+  </si>
+  <si>
+    <t>Havant Hearing Centre, The Courthouse, Elmleigh Road, Havant, PO9 2AL</t>
+  </si>
+  <si>
+    <t>Exeter Combined Court, Southernhay Gardens, Exeter, EX1 1UH</t>
+  </si>
+  <si>
+    <t>Glasgow Tribunal Centre, Atlantic Quay, 20 York Street, Glasgow, G2 8GT</t>
+  </si>
+  <si>
+    <t>Ground Floor, Block C, Caledonian House, Greenmarket, Dundee, DD1 4QG</t>
+  </si>
+  <si>
+    <t>4th Floor, City Exchange, 11 Albion Street, Leeds, LS1 5ES</t>
+  </si>
+  <si>
+    <t>Wilberforce Court, Alfred Gelder Street, Hull, HU1 1UY</t>
+  </si>
+  <si>
+    <t>The Law Courts, 50 West Bar, Sheffield, S3 8PH</t>
+  </si>
+  <si>
+    <t>Montague Court, 101 London Road, West Croydon, London, CR0 2RF</t>
+  </si>
+  <si>
+    <t>1st Floor, Ashford House, County Square Shopping Centre, Ashford, TN23 1YB</t>
+  </si>
+  <si>
+    <t>Victory House, 30-34 Kingsway, London, WC2B 6EX</t>
+  </si>
+  <si>
+    <t>London (Central), 4th Floor Fox Court, 30 Brooke Street, London, EC1N 7RS</t>
+  </si>
+  <si>
+    <t>East London Tribunals, 2nd Floor Import Building, 2 Clove Crescent, London,E 14 2BE</t>
+  </si>
+  <si>
+    <t>Newcastle CFCTC, Barras Bridge, Newcastle upon Tyne, Tyne &amp; Wear, NE1 8QF</t>
+  </si>
+  <si>
+    <t>Victoria Square, Middlesbrough, TS1 2AS</t>
+  </si>
+  <si>
+    <t>Earl Grey Way, North Shields, NE29 6AR</t>
+  </si>
+  <si>
+    <t>North Shields</t>
+  </si>
+  <si>
+    <t>Manchester Employment Tribunals, Alexandra House, 14-22 The Parsonage, Manchester, M3 2JA</t>
+  </si>
+  <si>
+    <t>Employment Tribunals, Third Floor, Civil &amp; Family Court, 35 Vernon Street, Liverpool, L2 2BX</t>
+  </si>
+  <si>
+    <t>Carlisle Combined Court, Courts of Justice, Earl Street, Carlisle, Cumbria, CA1 1DJ</t>
+  </si>
+  <si>
+    <t>Carlisle Magistrates Court, The Court House, Rickergate, Carlisle, CA3 8 QH</t>
+  </si>
+  <si>
+    <t>Barrow Magistrates Court, Abbey Road, Barrow in Furness, Cumbria, LA14 5QX</t>
+  </si>
+  <si>
+    <t>Blackpool Magistrates Court, Civic Centre, Chapel Street, Blackpool, Lancashire, FY1 5DQ</t>
+  </si>
+  <si>
+    <t>Piccadilly Exchange, 2 Piccadilly Plaza, Mosley Street, Manchester, M1 4AH</t>
+  </si>
+  <si>
+    <t>The Lowry Theatre Complex, Pier 8, Salford Quays, Salford, M50 3AZ</t>
+  </si>
+  <si>
+    <t>The Lowry</t>
+  </si>
+  <si>
+    <t>Tribunal Hearing Centre, Nottingham Justice Centre, Carrington Street, Nottingham, NG2 1EE</t>
+  </si>
+  <si>
+    <t>Leicester Hearing Centre, 5a New Walk, Leicester, LE1 6TE</t>
+  </si>
+  <si>
+    <t>Lincoln Magistrates Court, 358 High Street, Lincoln, LN5 7QA</t>
+  </si>
+  <si>
+    <t>Boston Court House, 55 Norfolk Street, Boston, PE21 6PE</t>
+  </si>
+  <si>
+    <t>Midlands West Employment Tribunal, Centre City Tower, 5-7 Hill Street, Birmingham, West Midlands, B5 4UU</t>
+  </si>
+  <si>
+    <t>Stoke-on-Trent Combined Court, Bethesda Street, Hanley, Stoke-on-Trent, T1 3BP</t>
+  </si>
+  <si>
+    <t>Telford Magistrates Court, Telford Square, Malinsgate, Telford, Shropshire, TF3 4HX</t>
+  </si>
+  <si>
+    <r>
+      <t>Wales Employment Tribunal, 3</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Floor, Cardiff Magistrates’ Court, Fitzalan Place, Cardiff, CF24 0RZ</t>
+    </r>
+  </si>
+  <si>
+    <t>3rd Floor, Radius House, 51 Clarendon Road, Watford, WD17 1HP</t>
+  </si>
+  <si>
+    <t>Reading Tribunal Hearing Centre 2nd Floor, 30-31 Friar Street, Reading, RG1 1DX</t>
+  </si>
+  <si>
+    <t>Amersham Law Courts King George V Road, Amersham, HP6 5AJ</t>
+  </si>
+  <si>
+    <t>Aylesbury Crown Court, Walton Street, Aylesbury, HP21 7FT</t>
+  </si>
+  <si>
+    <t>Huntingdon Law Courts Walden Rd, Huntingdon, PE29 3DW</t>
+  </si>
+  <si>
+    <t>Bedford County Court and Family Court, Shire Hall, 3 St Paul's Square, Bedford, MK40 1SQ</t>
+  </si>
+  <si>
+    <t>Cambridge County Court and Family Court, 197 East Road, Cambridge, CB1 1BA</t>
+  </si>
+  <si>
+    <t>Bury St Edmunds County Court and Family Court, Triton House, St Andrew's Street, North, Bury St. Edmunds, IP33 1TR</t>
+  </si>
+  <si>
+    <t>Norwich Magistrates' Court and Family Court, Bishopgate, Norwich, NR3 1UP</t>
+  </si>
+  <si>
+    <t>Peterborough</t>
+  </si>
+  <si>
+    <t>Peterborough nightingale Court Knights’ Chamber and Visitor Centre, Bishop’s, Palace, Peterborough Cathedral, Peterborough, PE1 1XZ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -609,8 +773,42 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
-      <sz val="12"/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -631,7 +829,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -646,31 +844,7 @@
       <right style="hair">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -678,21 +852,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1009,333 +1184,334 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D604D91D-6235-9B48-BBC4-151657576CA7}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="60.1640625" customWidth="1"/>
+    <col min="1" max="1" width="27" style="1" customWidth="1"/>
+    <col min="2" max="2" width="112.5" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B4" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="B14" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="B21" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="B22" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="B26" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B28" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="B28" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B31" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="B31" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1348,53 +1524,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DABB460-37E4-BC4E-8C69-80DBA2CDCD9B}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="61.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="113" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="B2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="B2" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="B3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="B3" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="B4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="B4" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>182</v>
       </c>
     </row>
@@ -1411,29 +1588,30 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="2" max="2" width="60.83203125" customWidth="1"/>
+    <col min="1" max="1" width="26.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="113.6640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>105</v>
       </c>
@@ -1441,507 +1619,507 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" spans="1:2" ht="22" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B14" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="B14" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" s="3" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B66" s="9" t="s">
         <v>168</v>
       </c>
     </row>
@@ -1952,128 +2130,137 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E10867F8-B593-C74C-AEF3-18F126ED778C}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.83203125" customWidth="1"/>
-    <col min="2" max="2" width="61.6640625" customWidth="1"/>
+    <col min="1" max="1" width="25.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="134" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="B2" s="8" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="B3" s="8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="B4" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="B6" s="8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+      <c r="B7" s="8" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="B8" s="8" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+      <c r="B11" s="8" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+      <c r="B12" s="8" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>177</v>
+      <c r="B14" s="10" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -2089,69 +2276,70 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="2" max="2" width="61" customWidth="1"/>
+    <col min="1" max="1" width="26.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="113.33203125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B4" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B6" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>48</v>
       </c>
@@ -2172,49 +2360,50 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="62" customWidth="1"/>
+    <col min="1" max="1" width="26" style="1" customWidth="1"/>
+    <col min="2" max="2" width="112.83203125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B4" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2231,49 +2420,50 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" customWidth="1"/>
-    <col min="2" max="2" width="61.83203125" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="112.6640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B3" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2290,41 +2480,42 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" customWidth="1"/>
-    <col min="2" max="2" width="61.5" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="113" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B2" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B3" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2335,43 +2526,44 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF6839BC-E7B7-4041-B35B-75697A68FCA7}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" customWidth="1"/>
-    <col min="2" max="2" width="61.33203125" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="113.6640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>60</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>61</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>62</v>
       </c>
@@ -2379,23 +2571,23 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>63</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>64</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>65</v>
       </c>
@@ -2403,7 +2595,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>66</v>
       </c>
@@ -2411,7 +2603,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>67</v>
       </c>
@@ -2419,7 +2611,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>68</v>
       </c>
@@ -2427,31 +2619,31 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>69</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>70</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>71</v>
       </c>
@@ -2459,7 +2651,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>72</v>
       </c>
@@ -2467,12 +2659,20 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>73</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -2488,101 +2688,102 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="2" max="2" width="60.33203125" customWidth="1"/>
+    <col min="1" max="1" width="26.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="113.1640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B3" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B6" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B7" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+      <c r="B10" s="8" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="8" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>83</v>
       </c>
@@ -2590,7 +2791,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>84</v>
       </c>
@@ -2598,7 +2799,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>85</v>
       </c>
@@ -2606,11 +2807,11 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2627,90 +2828,91 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" customWidth="1"/>
-    <col min="2" max="2" width="61.33203125" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="114.1640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B3" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B9" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="B9" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B10" t="s">
-        <v>94</v>
+      <c r="B10" s="1" t="s">
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -2720,43 +2922,44 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249D15DB-9300-074E-8219-2940BCE455E3}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="2" max="2" width="61.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="112.6640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>97</v>
       </c>
@@ -2764,53 +2967,64 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B7" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B8" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>103</v>
       </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
topped up unit test coverage
</commit_message>
<xml_diff>
--- a/src/main/resources/venueAddressValues.xlsx
+++ b/src/main/resources/venueAddressValues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rabab/HMCTS/ethos-repl-docmosis-service/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03AE8524-6EF0-CD4E-8BBF-60C50600BCA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374BE18D-EB4E-AE4E-8B39-D849E1D6226C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19460" activeTab="9" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
   </bookViews>
   <sheets>
     <sheet name="Bristol" sheetId="3" r:id="rId1"/>
@@ -852,7 +852,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -868,6 +868,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1184,7 +1186,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D604D91D-6235-9B48-BBC4-151657576CA7}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -1522,9 +1524,9 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DABB460-37E4-BC4E-8C69-80DBA2CDCD9B}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -1543,35 +1545,39 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>191</v>
-      </c>
+    <row r="2" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>182</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added validation of responseStruckOut
</commit_message>
<xml_diff>
--- a/src/main/resources/venueAddressValues.xlsx
+++ b/src/main/resources/venueAddressValues.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://justiceuk-my.sharepoint.com/personal/thomas_hart_justice_gov_uk/Documents/__Project team/ECM/Hearing rooms/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\THART\OneDrive - Ministry of Justice\__Project team\ECM\Hearing rooms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{4A606AF5-2602-4C5E-9100-BBBCE9FA0D52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CD7BC08D-FC42-4E10-8B72-27699E2FB101}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{6B76E839-C9C8-4B0F-9E08-05AC616E2D24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{51697465-B877-4D60-95AF-6CE689B6EDE8}"/>
   <bookViews>
-    <workbookView xWindow="-4476" yWindow="864" windowWidth="17280" windowHeight="8964" activeTab="9" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
+    <workbookView xWindow="41808" yWindow="2268" windowWidth="17280" windowHeight="8964" activeTab="9" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
   </bookViews>
   <sheets>
     <sheet name="Bristol" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="267">
   <si>
     <t>Leeds</t>
   </si>
@@ -851,6 +851,15 @@
   </si>
   <si>
     <t xml:space="preserve">Kirkcudbright Sheriff Court </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OET Scotland </t>
+  </si>
+  <si>
+    <t>Ground Floor, Endeavour House, 1 Greenmarket, Dundee, DD1 4QB</t>
+  </si>
+  <si>
+    <t>Tribunal Service</t>
   </si>
 </sst>
 </file>
@@ -945,7 +954,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -968,6 +977,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1623,10 +1635,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DABB460-37E4-BC4E-8C69-80DBA2CDCD9B}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1806,6 +1818,22 @@
       </c>
       <c r="B22" s="13" t="s">
         <v>256</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -3269,6 +3297,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E98ADB2028FC4F43824F86666CC83903" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ff47f26d8558bca2ac2c896a7e751c25">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bc19a69a-bda7-4614-8881-f2ac618cff8e" xmlns:ns4="02128cc3-8226-4d54-9246-100bb62c9520" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="63ef4ea587d9ab0193671c85d2373b1f" ns3:_="" ns4:_="">
     <xsd:import namespace="bc19a69a-bda7-4614-8881-f2ac618cff8e"/>
@@ -3485,7 +3519,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -3494,13 +3528,16 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E254D28-D3D4-49BF-9139-FF4FDEF467DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00A2FE85-4E03-4320-929A-8E66617AF346}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3519,19 +3556,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E21D230-F0FF-46F1-8C9B-DF853E5491B6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E254D28-D3D4-49BF-9139-FF4FDEF467DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added allocated hearing and updated data model
</commit_message>
<xml_diff>
--- a/src/main/resources/venueAddressValues.xlsx
+++ b/src/main/resources/venueAddressValues.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\THART\OneDrive - Ministry of Justice\__Project team\ECM\Hearing rooms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://justiceuk-my.sharepoint.com/personal/thomas_hart_justice_gov_uk/Documents/__Project team/ECM/Hearing rooms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{6B76E839-C9C8-4B0F-9E08-05AC616E2D24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{51697465-B877-4D60-95AF-6CE689B6EDE8}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{D8FDBA84-7697-41E8-8F2E-8A531EA35630}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E6EA0503-B2FF-4379-BAEC-343576E1F4EC}"/>
   <bookViews>
-    <workbookView xWindow="41808" yWindow="2268" windowWidth="17280" windowHeight="8964" activeTab="9" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
   </bookViews>
   <sheets>
     <sheet name="Bristol" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="266">
   <si>
     <t>Leeds</t>
   </si>
@@ -853,13 +853,10 @@
     <t xml:space="preserve">Kirkcudbright Sheriff Court </t>
   </si>
   <si>
-    <t xml:space="preserve">OET Scotland </t>
-  </si>
-  <si>
-    <t>Ground Floor, Endeavour House, 1 Greenmarket, Dundee, DD1 4QB</t>
-  </si>
-  <si>
-    <t>Tribunal Service</t>
+    <t>Hull Combined Court Centre</t>
+  </si>
+  <si>
+    <t>Lowgate, Hull, HU1 2EZ</t>
   </si>
 </sst>
 </file>
@@ -954,7 +951,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -977,9 +974,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1635,10 +1629,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DABB460-37E4-BC4E-8C69-80DBA2CDCD9B}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1818,22 +1812,6 @@
       </c>
       <c r="B22" s="13" t="s">
         <v>256</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -2535,10 +2513,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5FBCDA9-DEB7-ED42-9C1E-52C20E93783E}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -2610,6 +2588,14 @@
       </c>
       <c r="B8" s="4" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -3303,6 +3289,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E98ADB2028FC4F43824F86666CC83903" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ff47f26d8558bca2ac2c896a7e751c25">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bc19a69a-bda7-4614-8881-f2ac618cff8e" xmlns:ns4="02128cc3-8226-4d54-9246-100bb62c9520" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="63ef4ea587d9ab0193671c85d2373b1f" ns3:_="" ns4:_="">
     <xsd:import namespace="bc19a69a-bda7-4614-8881-f2ac618cff8e"/>
@@ -3519,15 +3514,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E254D28-D3D4-49BF-9139-FF4FDEF467DC}">
   <ds:schemaRefs>
@@ -3538,6 +3524,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E21D230-F0FF-46F1-8C9B-DF853E5491B6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00A2FE85-4E03-4320-929A-8E66617AF346}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3554,12 +3548,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E21D230-F0FF-46F1-8C9B-DF853E5491B6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated venue address values
</commit_message>
<xml_diff>
--- a/src/main/resources/venueAddressValues.xlsx
+++ b/src/main/resources/venueAddressValues.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://justiceuk-my.sharepoint.com/personal/thomas_hart_justice_gov_uk/Documents/__Project team/ECM/Hearing rooms/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\THART\OneDrive - Ministry of Justice\__Project team\ECM\Hearing rooms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{D8FDBA84-7697-41E8-8F2E-8A531EA35630}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E6EA0503-B2FF-4379-BAEC-343576E1F4EC}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{D8FDBA84-7697-41E8-8F2E-8A531EA35630}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1BC5155E-0977-4087-9C29-359673C44E89}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="10" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
   </bookViews>
   <sheets>
     <sheet name="Bristol" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="268">
   <si>
     <t>Leeds</t>
   </si>
@@ -857,6 +857,12 @@
   </si>
   <si>
     <t>Lowgate, Hull, HU1 2EZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cardiff SSCS </t>
+  </si>
+  <si>
+    <t>Eastgate House, 35-43 Newport Rd, Cardiff CF24 0AB</t>
   </si>
 </sst>
 </file>
@@ -1825,10 +1831,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08CEAEC1-EF84-7E4A-89B0-924FD73F7AD5}">
-  <dimension ref="A1:B66"/>
+  <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -2364,6 +2370,14 @@
       </c>
       <c r="B66" s="9" t="s">
         <v>168</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -2515,7 +2529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5FBCDA9-DEB7-ED42-9C1E-52C20E93783E}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -3283,21 +3297,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E98ADB2028FC4F43824F86666CC83903" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ff47f26d8558bca2ac2c896a7e751c25">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bc19a69a-bda7-4614-8881-f2ac618cff8e" xmlns:ns4="02128cc3-8226-4d54-9246-100bb62c9520" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="63ef4ea587d9ab0193671c85d2373b1f" ns3:_="" ns4:_="">
     <xsd:import namespace="bc19a69a-bda7-4614-8881-f2ac618cff8e"/>
@@ -3514,24 +3513,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E254D28-D3D4-49BF-9139-FF4FDEF467DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E21D230-F0FF-46F1-8C9B-DF853E5491B6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00A2FE85-4E03-4320-929A-8E66617AF346}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3548,4 +3545,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E21D230-F0FF-46F1-8C9B-DF853E5491B6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E254D28-D3D4-49BF-9139-FF4FDEF467DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Hotfix for venues and ct
</commit_message>
<xml_diff>
--- a/src/main/resources/venueAddressValues.xlsx
+++ b/src/main/resources/venueAddressValues.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\THART\OneDrive - Ministry of Justice\__Project team\ECM\Hearing rooms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://justiceuk-my.sharepoint.com/personal/thomas_hart_justice_gov_uk/Documents/__Project team/ECM/Hearing rooms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{D8FDBA84-7697-41E8-8F2E-8A531EA35630}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B2DCD2A2-A206-48DC-8479-0EBA543ED335}"/>
+  <xr:revisionPtr revIDLastSave="83" documentId="8_{F53D74CB-525D-46F0-9264-C32A22C09D13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5B66F9D5-F7DE-4DCB-B124-C48A7A0BB28D}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="13164" windowHeight="11880" firstSheet="5" activeTab="9" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16896" firstSheet="6" activeTab="10" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
   </bookViews>
   <sheets>
     <sheet name="Bristol" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="289">
   <si>
     <t>Leeds</t>
   </si>
@@ -875,6 +875,80 @@
   </si>
   <si>
     <t>Ground Floor, Endeavour House, 1 Greenmarket, Dundee, DD1 4QB</t>
+  </si>
+  <si>
+    <t>Y Lanfa, Trefechan, Aberystwyth, SY23 1AS</t>
+  </si>
+  <si>
+    <t>Llanberis Road, Caernarfon, LL55 2DF</t>
+  </si>
+  <si>
+    <t>2 Park Street, Cardiff, CF10 1ET</t>
+  </si>
+  <si>
+    <t>The Law Courts, Cathays Park, Cardiff, CF10 3PG</t>
+  </si>
+  <si>
+    <t>3rd Floor, Cardiff Magistrates’ Court, Fitzalan Place, Cardiff, CF24 0RZ</t>
+  </si>
+  <si>
+    <t>The Hearing Centre, Hill House, Picton Terrace, Carmarthen, SA31 3BT</t>
+  </si>
+  <si>
+    <t>Penffynnon, Hawthorn Rise, Haverfordwest, SA61 2AX</t>
+  </si>
+  <si>
+    <t>The Court House, Conwy Road, Llandudno, LL30 1GA</t>
+  </si>
+  <si>
+    <t>Town Hall Square, Llanelli, SA15 3AW</t>
+  </si>
+  <si>
+    <t>Law Courts, Mold, CH7 1AE</t>
+  </si>
+  <si>
+    <t>The Courthouse, Courthouse Street, Pontypridd, CF37 1JR</t>
+  </si>
+  <si>
+    <t>Harbourside Road, Port Talbot, SA13 1SB</t>
+  </si>
+  <si>
+    <t>Victoria Road, Prestatyn, LL19 7TE</t>
+  </si>
+  <si>
+    <r>
+      <t>Caravella House, Quay West, Quay Parade</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Swansea, SA1 1SP</t>
+    </r>
+  </si>
+  <si>
+    <t>Grove Place, Swansea, SA1 5DB</t>
+  </si>
+  <si>
+    <t>Mansion House, 24 Severn Street, Welshpool, SY21 7UX</t>
+  </si>
+  <si>
+    <t>The Law Courts, Bodhyfryd, Wrexham, LL12 7BP</t>
   </si>
 </sst>
 </file>
@@ -1649,7 +1723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DABB460-37E4-BC4E-8C69-80DBA2CDCD9B}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -1861,14 +1935,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08CEAEC1-EF84-7E4A-89B0-924FD73F7AD5}">
   <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="113.69921875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.8984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="36.19921875" style="1" customWidth="1"/>
     <col min="3" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
@@ -1901,7 +1975,7 @@
         <v>106</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>106</v>
+        <v>272</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -1933,7 +2007,7 @@
         <v>110</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>110</v>
+        <v>273</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -1949,7 +2023,7 @@
         <v>112</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>112</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -1957,7 +2031,7 @@
         <v>113</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>113</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -2013,7 +2087,7 @@
         <v>120</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>120</v>
+        <v>277</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -2101,7 +2175,7 @@
         <v>131</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>131</v>
+        <v>278</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -2157,7 +2231,7 @@
         <v>138</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>138</v>
+        <v>279</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
@@ -2173,7 +2247,7 @@
         <v>140</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>140</v>
+        <v>280</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
@@ -2205,7 +2279,7 @@
         <v>144</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>144</v>
+        <v>281</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
@@ -2261,7 +2335,7 @@
         <v>151</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>151</v>
+        <v>282</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
@@ -2269,7 +2343,7 @@
         <v>152</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>152</v>
+        <v>283</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
@@ -2277,7 +2351,7 @@
         <v>153</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>153</v>
+        <v>284</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
@@ -2317,7 +2391,7 @@
         <v>158</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>158</v>
+        <v>285</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
@@ -2333,7 +2407,7 @@
         <v>160</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>160</v>
+        <v>286</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
@@ -2365,7 +2439,7 @@
         <v>164</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>164</v>
+        <v>276</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
@@ -2373,7 +2447,7 @@
         <v>165</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>165</v>
+        <v>287</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
@@ -2389,7 +2463,7 @@
         <v>167</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>167</v>
+        <v>288</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
@@ -2410,6 +2484,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3325,6 +3400,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E98ADB2028FC4F43824F86666CC83903" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ff47f26d8558bca2ac2c896a7e751c25">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bc19a69a-bda7-4614-8881-f2ac618cff8e" xmlns:ns4="02128cc3-8226-4d54-9246-100bb62c9520" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="63ef4ea587d9ab0193671c85d2373b1f" ns3:_="" ns4:_="">
     <xsd:import namespace="bc19a69a-bda7-4614-8881-f2ac618cff8e"/>
@@ -3541,15 +3625,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3557,6 +3632,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E21D230-F0FF-46F1-8C9B-DF853E5491B6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00A2FE85-4E03-4320-929A-8E66617AF346}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3575,14 +3658,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E21D230-F0FF-46F1-8C9B-DF853E5491B6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E254D28-D3D4-49BF-9139-FF4FDEF467DC}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
ECM-214 Update venue address for Hull Combined Court Centre
</commit_message>
<xml_diff>
--- a/src/main/resources/venueAddressValues.xlsx
+++ b/src/main/resources/venueAddressValues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://justiceuk-my.sharepoint.com/personal/thomas_hart_justice_gov_uk/Documents/__Project team/ECM/Hearing rooms/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesturnbull/code/hmcts/ecm/ethos-repl-docmosis-service/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="8_{F53D74CB-525D-46F0-9264-C32A22C09D13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5B66F9D5-F7DE-4DCB-B124-C48A7A0BB28D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492AD93E-1B95-FC40-A4AA-A8F719F93D26}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16896" firstSheet="6" activeTab="10" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
+    <workbookView xWindow="2840" yWindow="1740" windowWidth="30940" windowHeight="16900" activeTab="1" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
   </bookViews>
   <sheets>
     <sheet name="Bristol" sheetId="3" r:id="rId1"/>
@@ -856,9 +856,6 @@
     <t>Hull Combined Court Centre</t>
   </si>
   <si>
-    <t>Lowgate, Hull, HU1 2EZ</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cardiff SSCS </t>
   </si>
   <si>
@@ -949,6 +946,9 @@
   </si>
   <si>
     <t>The Law Courts, Bodhyfryd, Wrexham, LL12 7BP</t>
+  </si>
+  <si>
+    <t>Hull Combined Court Centre, Lowgate, Hull, HU1 2EZ</t>
   </si>
 </sst>
 </file>
@@ -1387,14 +1387,14 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" style="1" customWidth="1"/>
     <col min="2" max="2" width="112.5" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.796875" style="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -1482,7 +1482,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -1506,7 +1506,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>35</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>36</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>37</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>38</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>39</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>40</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>41</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>42</v>
       </c>
@@ -1727,14 +1727,14 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.19921875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="113" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.796875" style="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1742,11 +1742,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>179</v>
       </c>
@@ -1754,7 +1754,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>261</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>234</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>180</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>181</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>262</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>178</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>257</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>263</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>259</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>250</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>240</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>237</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>242</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>252</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>244</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>254</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>246</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>248</v>
       </c>
@@ -1898,7 +1898,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>255</v>
       </c>
@@ -1906,20 +1906,20 @@
         <v>256</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B23" s="1" t="s">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -1935,18 +1935,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08CEAEC1-EF84-7E4A-89B0-924FD73F7AD5}">
   <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.8984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="36.19921875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.796875" style="1"/>
+    <col min="1" max="1" width="22.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="36.1640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>104</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>105</v>
       </c>
@@ -1970,15 +1970,15 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>106</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>107</v>
       </c>
@@ -1986,7 +1986,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>108</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>109</v>
       </c>
@@ -2002,15 +2002,15 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>110</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>111</v>
       </c>
@@ -2018,23 +2018,23 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>113</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>114</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>115</v>
       </c>
@@ -2050,7 +2050,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="19.8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" ht="22" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>116</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>117</v>
       </c>
@@ -2066,7 +2066,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>118</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>119</v>
       </c>
@@ -2082,15 +2082,15 @@
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>120</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>121</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>122</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>123</v>
       </c>
@@ -2114,7 +2114,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>124</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>125</v>
       </c>
@@ -2130,7 +2130,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>126</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>127</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>128</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>129</v>
       </c>
@@ -2162,7 +2162,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>130</v>
       </c>
@@ -2170,15 +2170,15 @@
         <v>130</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>131</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>132</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>133</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>134</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>135</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>136</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>137</v>
       </c>
@@ -2226,15 +2226,15 @@
         <v>137</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>138</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>139</v>
       </c>
@@ -2242,15 +2242,15 @@
         <v>139</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>140</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>141</v>
       </c>
@@ -2258,7 +2258,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>142</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>143</v>
       </c>
@@ -2274,15 +2274,15 @@
         <v>143</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>144</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>145</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>146</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>147</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>148</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>149</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>150</v>
       </c>
@@ -2330,31 +2330,31 @@
         <v>150</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>151</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>152</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>153</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>154</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>155</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>156</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>157</v>
       </c>
@@ -2386,15 +2386,15 @@
         <v>157</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>158</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>159</v>
       </c>
@@ -2402,15 +2402,15 @@
         <v>159</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>160</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>161</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>162</v>
       </c>
@@ -2426,7 +2426,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>163</v>
       </c>
@@ -2434,23 +2434,23 @@
         <v>163</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>165</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>166</v>
       </c>
@@ -2458,15 +2458,15 @@
         <v>166</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>167</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>168</v>
       </c>
@@ -2474,12 +2474,12 @@
         <v>168</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -2496,14 +2496,14 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.796875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="134" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.796875" style="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>169</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>170</v>
       </c>
@@ -2527,7 +2527,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>74</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>171</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>89</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>90</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>172</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>51</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>173</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>174</v>
       </c>
@@ -2591,7 +2591,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>175</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>176</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>177</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>231</v>
       </c>
@@ -2632,18 +2632,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5FBCDA9-DEB7-ED42-9C1E-52C20E93783E}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="113.296875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.796875" style="1"/>
+    <col min="2" max="2" width="113.33203125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -2651,7 +2651,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>43</v>
       </c>
@@ -2659,7 +2659,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>44</v>
       </c>
@@ -2667,7 +2667,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>45</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>46</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>47</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>48</v>
       </c>
@@ -2707,12 +2707,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>264</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>265</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -2728,14 +2728,14 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" style="1" customWidth="1"/>
-    <col min="2" max="2" width="112.796875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.796875" style="1"/>
+    <col min="2" max="2" width="112.83203125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>49</v>
       </c>
@@ -2751,7 +2751,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>50</v>
       </c>
@@ -2759,7 +2759,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>51</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>52</v>
       </c>
@@ -2788,14 +2788,14 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.69921875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="112.69921875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.796875" style="1"/>
+    <col min="1" max="1" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="112.6640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -2803,7 +2803,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>53</v>
       </c>
@@ -2811,7 +2811,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>54</v>
       </c>
@@ -2819,7 +2819,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>55</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>56</v>
       </c>
@@ -2848,14 +2848,14 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.69921875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="113" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.796875" style="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>57</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>58</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>59</v>
       </c>
@@ -2900,14 +2900,14 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="113.69921875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.796875" style="1"/>
+    <col min="1" max="1" width="26.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="113.6640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>60</v>
       </c>
@@ -2923,7 +2923,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>61</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>62</v>
       </c>
@@ -2939,7 +2939,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>63</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>64</v>
       </c>
@@ -2955,7 +2955,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>65</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>66</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>67</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>68</v>
       </c>
@@ -2987,7 +2987,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>69</v>
       </c>
@@ -2995,7 +2995,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>1</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>70</v>
       </c>
@@ -3011,7 +3011,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>71</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>72</v>
       </c>
@@ -3027,7 +3027,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>73</v>
       </c>
@@ -3035,7 +3035,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>213</v>
       </c>
@@ -3056,14 +3056,14 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="113.19921875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.796875" style="1"/>
+    <col min="2" max="2" width="113.1640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -3071,7 +3071,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>74</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>75</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>76</v>
       </c>
@@ -3095,7 +3095,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>77</v>
       </c>
@@ -3103,7 +3103,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>78</v>
       </c>
@@ -3111,7 +3111,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>79</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>51</v>
       </c>
@@ -3127,7 +3127,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>80</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>81</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>82</v>
       </c>
@@ -3151,7 +3151,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>83</v>
       </c>
@@ -3159,7 +3159,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>84</v>
       </c>
@@ -3167,7 +3167,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>85</v>
       </c>
@@ -3175,7 +3175,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>86</v>
       </c>
@@ -3196,14 +3196,14 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="114.19921875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.796875" style="1"/>
+    <col min="1" max="1" width="26.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="114.1640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -3211,7 +3211,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>87</v>
       </c>
@@ -3219,7 +3219,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>88</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>89</v>
       </c>
@@ -3235,7 +3235,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>90</v>
       </c>
@@ -3243,7 +3243,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>91</v>
       </c>
@@ -3251,7 +3251,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>78</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>92</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>93</v>
       </c>
@@ -3275,7 +3275,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>94</v>
       </c>
@@ -3296,14 +3296,14 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="112.69921875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.796875" style="1"/>
+    <col min="2" max="2" width="112.6640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -3311,7 +3311,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>95</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>96</v>
       </c>
@@ -3327,7 +3327,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>97</v>
       </c>
@@ -3335,7 +3335,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>98</v>
       </c>
@@ -3343,7 +3343,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>99</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>100</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>101</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>102</v>
       </c>
@@ -3375,7 +3375,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>103</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>204</v>
       </c>
@@ -3391,7 +3391,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
     </row>
   </sheetData>
@@ -3400,15 +3400,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E98ADB2028FC4F43824F86666CC83903" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ff47f26d8558bca2ac2c896a7e751c25">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bc19a69a-bda7-4614-8881-f2ac618cff8e" xmlns:ns4="02128cc3-8226-4d54-9246-100bb62c9520" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="63ef4ea587d9ab0193671c85d2373b1f" ns3:_="" ns4:_="">
     <xsd:import namespace="bc19a69a-bda7-4614-8881-f2ac618cff8e"/>
@@ -3625,6 +3616,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3632,14 +3632,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E21D230-F0FF-46F1-8C9B-DF853E5491B6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00A2FE85-4E03-4320-929A-8E66617AF346}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3658,6 +3650,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E21D230-F0FF-46F1-8C9B-DF853E5491B6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E254D28-D3D4-49BF-9139-FF4FDEF467DC}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Update Watford hearing venue address
</commit_message>
<xml_diff>
--- a/src/main/resources/venueAddressValues.xlsx
+++ b/src/main/resources/venueAddressValues.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesturnbull/code/hmcts/ecm/ethos-repl-docmosis-service/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesturnbull/code/local/ethos-repl-docmosis-service/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B39E46-F7FC-3C46-9687-D12B605FA113}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C94DDB-F331-724F-9CD9-C4984C24BC05}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2840" yWindow="1740" windowWidth="30940" windowHeight="16900" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
+    <workbookView xWindow="75320" yWindow="360" windowWidth="35820" windowHeight="17980" activeTab="11" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
   </bookViews>
   <sheets>
     <sheet name="Bristol" sheetId="3" r:id="rId1"/>
@@ -727,9 +727,6 @@
     </r>
   </si>
   <si>
-    <t>3rd Floor, Radius House, 51 Clarendon Road, Watford, WD17 1HP</t>
-  </si>
-  <si>
     <t>Reading Tribunal Hearing Centre 2nd Floor, 30-31 Friar Street, Reading, RG1 1DX</t>
   </si>
   <si>
@@ -955,6 +952,9 @@
   </si>
   <si>
     <t>Teesside Justice Centre, Victoria Square, Middlesbrough, Cleveland, TS1 2AS</t>
+  </si>
+  <si>
+    <t>2rd Floor, Radius House, 51 Clarendon Road, Watford, WD17 1HP</t>
   </si>
 </sst>
 </file>
@@ -1382,7 +1382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D604D91D-6235-9B48-BBC4-151657576CA7}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -1755,18 +1755,18 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>234</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1787,10 +1787,10 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1803,122 +1803,122 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>257</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>259</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="B13" s="12" t="s">
         <v>250</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="B14" s="12" t="s">
         <v>240</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="B16" s="12" t="s">
         <v>242</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="B17" s="12" t="s">
         <v>252</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>244</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="B20" s="12" t="s">
         <v>246</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="B21" s="12" t="s">
         <v>248</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="B22" s="12" t="s">
         <v>255</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>267</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>269</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -1974,7 +1974,7 @@
         <v>106</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2006,7 +2006,7 @@
         <v>110</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2022,7 +2022,7 @@
         <v>112</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2030,7 +2030,7 @@
         <v>113</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2086,7 +2086,7 @@
         <v>120</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2174,7 +2174,7 @@
         <v>131</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2230,7 +2230,7 @@
         <v>138</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2246,7 +2246,7 @@
         <v>140</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -2278,7 +2278,7 @@
         <v>144</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2334,7 +2334,7 @@
         <v>151</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2342,7 +2342,7 @@
         <v>152</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2350,7 +2350,7 @@
         <v>153</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2390,7 +2390,7 @@
         <v>158</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -2406,7 +2406,7 @@
         <v>160</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -2438,7 +2438,7 @@
         <v>164</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -2446,7 +2446,7 @@
         <v>165</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -2462,7 +2462,7 @@
         <v>167</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -2475,10 +2475,10 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -2491,8 +2491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E10867F8-B593-C74C-AEF3-18F126ED778C}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2515,7 +2515,7 @@
         <v>169</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2523,7 +2523,7 @@
         <v>170</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2531,7 +2531,7 @@
         <v>74</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2547,7 +2547,7 @@
         <v>89</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2555,7 +2555,7 @@
         <v>90</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2563,7 +2563,7 @@
         <v>172</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2587,7 +2587,7 @@
         <v>174</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2595,7 +2595,7 @@
         <v>175</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2611,15 +2611,15 @@
         <v>177</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>222</v>
+        <v>290</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>231</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -2708,10 +2708,10 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -3392,10 +3392,10 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>289</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -3404,21 +3404,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E98ADB2028FC4F43824F86666CC83903" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ff47f26d8558bca2ac2c896a7e751c25">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bc19a69a-bda7-4614-8881-f2ac618cff8e" xmlns:ns4="02128cc3-8226-4d54-9246-100bb62c9520" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="63ef4ea587d9ab0193671c85d2373b1f" ns3:_="" ns4:_="">
     <xsd:import namespace="bc19a69a-bda7-4614-8881-f2ac618cff8e"/>
@@ -3635,24 +3620,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E254D28-D3D4-49BF-9139-FF4FDEF467DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E21D230-F0FF-46F1-8C9B-DF853E5491B6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00A2FE85-4E03-4320-929A-8E66617AF346}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3669,4 +3652,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E21D230-F0FF-46F1-8C9B-DF853E5491B6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E254D28-D3D4-49BF-9139-FF4FDEF467DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix typo in address
</commit_message>
<xml_diff>
--- a/src/main/resources/venueAddressValues.xlsx
+++ b/src/main/resources/venueAddressValues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesturnbull/code/local/ethos-repl-docmosis-service/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C94DDB-F331-724F-9CD9-C4984C24BC05}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B913CEDE-088A-6F4E-BBCE-8AF07AF1AD24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="75320" yWindow="360" windowWidth="35820" windowHeight="17980" activeTab="11" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
   </bookViews>
@@ -954,7 +954,7 @@
     <t>Teesside Justice Centre, Victoria Square, Middlesbrough, Cleveland, TS1 2AS</t>
   </si>
   <si>
-    <t>2rd Floor, Radius House, 51 Clarendon Road, Watford, WD17 1HP</t>
+    <t>2nd Floor, Radius House, 51 Clarendon Road, Watford, WD17 1HP</t>
   </si>
 </sst>
 </file>
@@ -2492,7 +2492,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -3404,6 +3404,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E98ADB2028FC4F43824F86666CC83903" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ff47f26d8558bca2ac2c896a7e751c25">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bc19a69a-bda7-4614-8881-f2ac618cff8e" xmlns:ns4="02128cc3-8226-4d54-9246-100bb62c9520" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="63ef4ea587d9ab0193671c85d2373b1f" ns3:_="" ns4:_="">
     <xsd:import namespace="bc19a69a-bda7-4614-8881-f2ac618cff8e"/>
@@ -3620,22 +3635,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E254D28-D3D4-49BF-9139-FF4FDEF467DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E21D230-F0FF-46F1-8C9B-DF853E5491B6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00A2FE85-4E03-4320-929A-8E66617AF346}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3652,21 +3669,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E21D230-F0FF-46F1-8C9B-DF853E5491B6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E254D28-D3D4-49BF-9139-FF4FDEF467DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Venue Address change Nottingham Midlands East
</commit_message>
<xml_diff>
--- a/src/main/resources/venueAddressValues.xlsx
+++ b/src/main/resources/venueAddressValues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gauravchawla/Documents/tmp/ethos-repl-docmosis-service-latest/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEC0AE4-0F15-1E44-9DFD-7C24710F628F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1B2D6B-8012-704C-976A-F131217937EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20340" activeTab="10" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20260" activeTab="6" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
   </bookViews>
   <sheets>
     <sheet name="Bristol" sheetId="3" r:id="rId1"/>
@@ -680,9 +680,6 @@
     <t>The Lowry</t>
   </si>
   <si>
-    <t>Tribunal Hearing Centre, Nottingham Justice Centre, Carrington Street, Nottingham, NG2 1EE</t>
-  </si>
-  <si>
     <t>Leicester Hearing Centre, 5a New Walk, Leicester, LE1 6TE</t>
   </si>
   <si>
@@ -958,6 +955,9 @@
   </si>
   <si>
     <t>Columbus House, Langstone Business Park, Chepstow Road, Newport, NP18 2LX</t>
+  </si>
+  <si>
+    <t>Tribunal Hearing Centre, 50 Carrington Street, Nottingham, NG1 7FG</t>
   </si>
 </sst>
 </file>
@@ -1758,18 +1758,18 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>233</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1790,10 +1790,10 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1806,122 +1806,122 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>256</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>258</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="B13" s="12" t="s">
         <v>249</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="B14" s="12" t="s">
         <v>239</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="B16" s="12" t="s">
         <v>241</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="B17" s="12" t="s">
         <v>251</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>243</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="B20" s="12" t="s">
         <v>245</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="B21" s="12" t="s">
         <v>247</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="B22" s="12" t="s">
         <v>254</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -1937,7 +1937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08CEAEC1-EF84-7E4A-89B0-924FD73F7AD5}">
   <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
@@ -1977,7 +1977,7 @@
         <v>106</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2009,7 +2009,7 @@
         <v>110</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2025,7 +2025,7 @@
         <v>112</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2033,7 +2033,7 @@
         <v>113</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2057,7 +2057,7 @@
         <v>116</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2089,7 +2089,7 @@
         <v>120</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2177,7 +2177,7 @@
         <v>131</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2233,7 +2233,7 @@
         <v>138</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2249,7 +2249,7 @@
         <v>140</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -2281,7 +2281,7 @@
         <v>144</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2321,7 +2321,7 @@
         <v>149</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -2337,7 +2337,7 @@
         <v>151</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2345,7 +2345,7 @@
         <v>152</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2353,7 +2353,7 @@
         <v>153</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2393,7 +2393,7 @@
         <v>158</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -2409,7 +2409,7 @@
         <v>160</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -2441,7 +2441,7 @@
         <v>164</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -2449,7 +2449,7 @@
         <v>165</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -2465,7 +2465,7 @@
         <v>167</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -2478,10 +2478,10 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -2518,7 +2518,7 @@
         <v>169</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2526,7 +2526,7 @@
         <v>170</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2534,7 +2534,7 @@
         <v>74</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2550,7 +2550,7 @@
         <v>89</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2558,7 +2558,7 @@
         <v>90</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2566,7 +2566,7 @@
         <v>172</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2590,7 +2590,7 @@
         <v>174</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2598,7 +2598,7 @@
         <v>175</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2614,15 +2614,15 @@
         <v>177</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>230</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -2711,10 +2711,10 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -3054,8 +3054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0040410D-818E-3D4D-B0B2-19F9420DCC8F}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -3086,7 +3086,7 @@
         <v>75</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3110,7 +3110,7 @@
         <v>78</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3118,7 +3118,7 @@
         <v>79</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -3142,7 +3142,7 @@
         <v>81</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>214</v>
+        <v>291</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -3226,7 +3226,7 @@
         <v>88</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3274,7 +3274,7 @@
         <v>93</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -3282,7 +3282,7 @@
         <v>94</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -3395,10 +3395,10 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -3407,18 +3407,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3639,18 +3639,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E254D28-D3D4-49BF-9139-FF4FDEF467DC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E21D230-F0FF-46F1-8C9B-DF853E5491B6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E21D230-F0FF-46F1-8C9B-DF853E5491B6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E254D28-D3D4-49BF-9139-FF4FDEF467DC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
ECM-946 fix for master
</commit_message>
<xml_diff>
--- a/src/main/resources/venueAddressValues.xlsx
+++ b/src/main/resources/venueAddressValues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gauravchawla/Documents/tmp/ethos-repl-docmosis-service-latest/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEC0AE4-0F15-1E44-9DFD-7C24710F628F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0E8A4E-9549-7644-AC80-2E19A987ED4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20340" activeTab="10" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20260" activeTab="6" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
   </bookViews>
   <sheets>
     <sheet name="Bristol" sheetId="3" r:id="rId1"/>
@@ -680,9 +680,6 @@
     <t>The Lowry</t>
   </si>
   <si>
-    <t>Tribunal Hearing Centre, Nottingham Justice Centre, Carrington Street, Nottingham, NG2 1EE</t>
-  </si>
-  <si>
     <t>Leicester Hearing Centre, 5a New Walk, Leicester, LE1 6TE</t>
   </si>
   <si>
@@ -958,6 +955,9 @@
   </si>
   <si>
     <t>Columbus House, Langstone Business Park, Chepstow Road, Newport, NP18 2LX</t>
+  </si>
+  <si>
+    <t>Tribunal Hearing Centre, 50 Carrington Street, Nottingham, NG1 7FG</t>
   </si>
 </sst>
 </file>
@@ -1758,18 +1758,18 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>233</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1790,10 +1790,10 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1806,122 +1806,122 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>256</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>258</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="B13" s="12" t="s">
         <v>249</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="B14" s="12" t="s">
         <v>239</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="B16" s="12" t="s">
         <v>241</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="B17" s="12" t="s">
         <v>251</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>243</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="B20" s="12" t="s">
         <v>245</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="B21" s="12" t="s">
         <v>247</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="B22" s="12" t="s">
         <v>254</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -1937,7 +1937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08CEAEC1-EF84-7E4A-89B0-924FD73F7AD5}">
   <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
@@ -1977,7 +1977,7 @@
         <v>106</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2009,7 +2009,7 @@
         <v>110</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2025,7 +2025,7 @@
         <v>112</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2033,7 +2033,7 @@
         <v>113</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2057,7 +2057,7 @@
         <v>116</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2089,7 +2089,7 @@
         <v>120</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2177,7 +2177,7 @@
         <v>131</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2233,7 +2233,7 @@
         <v>138</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2249,7 +2249,7 @@
         <v>140</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -2281,7 +2281,7 @@
         <v>144</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2321,7 +2321,7 @@
         <v>149</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -2337,7 +2337,7 @@
         <v>151</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2345,7 +2345,7 @@
         <v>152</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2353,7 +2353,7 @@
         <v>153</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2393,7 +2393,7 @@
         <v>158</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -2409,7 +2409,7 @@
         <v>160</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -2441,7 +2441,7 @@
         <v>164</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -2449,7 +2449,7 @@
         <v>165</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -2465,7 +2465,7 @@
         <v>167</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -2478,10 +2478,10 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -2518,7 +2518,7 @@
         <v>169</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2526,7 +2526,7 @@
         <v>170</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2534,7 +2534,7 @@
         <v>74</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2550,7 +2550,7 @@
         <v>89</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2558,7 +2558,7 @@
         <v>90</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2566,7 +2566,7 @@
         <v>172</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2590,7 +2590,7 @@
         <v>174</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2598,7 +2598,7 @@
         <v>175</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2614,15 +2614,15 @@
         <v>177</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>230</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -2711,10 +2711,10 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -3054,8 +3054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0040410D-818E-3D4D-B0B2-19F9420DCC8F}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -3086,7 +3086,7 @@
         <v>75</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3110,7 +3110,7 @@
         <v>78</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3118,7 +3118,7 @@
         <v>79</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -3141,8 +3141,8 @@
       <c r="A10" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>214</v>
+      <c r="B10" s="1" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -3226,7 +3226,7 @@
         <v>88</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3274,7 +3274,7 @@
         <v>93</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -3282,7 +3282,7 @@
         <v>94</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -3395,10 +3395,10 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -3407,21 +3407,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E98ADB2028FC4F43824F86666CC83903" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ff47f26d8558bca2ac2c896a7e751c25">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bc19a69a-bda7-4614-8881-f2ac618cff8e" xmlns:ns4="02128cc3-8226-4d54-9246-100bb62c9520" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="63ef4ea587d9ab0193671c85d2373b1f" ns3:_="" ns4:_="">
     <xsd:import namespace="bc19a69a-bda7-4614-8881-f2ac618cff8e"/>
@@ -3638,24 +3623,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E254D28-D3D4-49BF-9139-FF4FDEF467DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E21D230-F0FF-46F1-8C9B-DF853E5491B6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00A2FE85-4E03-4320-929A-8E66617AF346}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3672,4 +3655,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E21D230-F0FF-46F1-8C9B-DF853E5491B6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E254D28-D3D4-49BF-9139-FF4FDEF467DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Venue Address Values updated
</commit_message>
<xml_diff>
--- a/src/main/resources/venueAddressValues.xlsx
+++ b/src/main/resources/venueAddressValues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harpreet.jhita/Projects/ethos-repl-docmosis-service/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tensaybulcha/Documents/GitHub/Reformed-ET/ethos-repl-docmosis-service/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F367472-9E9C-A947-B2B7-AC2E2CDFBF76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDAC5369-37CF-CF4B-A478-3D722A40B46A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="34280" windowHeight="28800" activeTab="10" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
+    <workbookView xWindow="56720" yWindow="500" windowWidth="30720" windowHeight="16420" activeTab="1" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
   </bookViews>
   <sheets>
     <sheet name="Bristol" sheetId="3" r:id="rId1"/>
@@ -860,9 +860,6 @@
     <t>Leeds Westgate</t>
   </si>
   <si>
-    <t>6 Westgate, Grace St, Leeds, LS1 2RP</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="14"/>
@@ -1322,6 +1319,9 @@
       </rPr>
       <t>, Eastgate House, 35-43 Newport Rd, Cardiff CF24 0AB</t>
     </r>
+  </si>
+  <si>
+    <t>2nd Floor, West Gate , 6 Grace Street, Leeds, LS1 2RP</t>
   </si>
 </sst>
 </file>
@@ -1458,9 +1458,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1498,7 +1498,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1604,7 +1604,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1746,7 +1746,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2308,8 +2308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08CEAEC1-EF84-7E4A-89B0-924FD73F7AD5}">
   <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2347,7 +2347,7 @@
         <v>106</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2379,7 +2379,7 @@
         <v>110</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2395,7 +2395,7 @@
         <v>112</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2403,7 +2403,7 @@
         <v>113</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2427,7 +2427,7 @@
         <v>116</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2459,7 +2459,7 @@
         <v>120</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2547,7 +2547,7 @@
         <v>131</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2603,7 +2603,7 @@
         <v>138</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2619,7 +2619,7 @@
         <v>140</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -2651,7 +2651,7 @@
         <v>144</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2691,7 +2691,7 @@
         <v>149</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -2707,7 +2707,7 @@
         <v>151</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2715,7 +2715,7 @@
         <v>152</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2723,7 +2723,7 @@
         <v>153</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2763,7 +2763,7 @@
         <v>158</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -2779,7 +2779,7 @@
         <v>160</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -2811,7 +2811,7 @@
         <v>164</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -2819,7 +2819,7 @@
         <v>165</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -2835,7 +2835,7 @@
         <v>167</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -2851,7 +2851,7 @@
         <v>262</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -3004,13 +3004,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5FBCDA9-DEB7-ED42-9C1E-52C20E93783E}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="113.33203125" style="1" customWidth="1"/>
     <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -3052,7 +3052,7 @@
         <v>273</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>274</v>
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3785,6 +3785,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E98ADB2028FC4F43824F86666CC83903" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ff47f26d8558bca2ac2c896a7e751c25">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bc19a69a-bda7-4614-8881-f2ac618cff8e" xmlns:ns4="02128cc3-8226-4d54-9246-100bb62c9520" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="63ef4ea587d9ab0193671c85d2373b1f" ns3:_="" ns4:_="">
     <xsd:import namespace="bc19a69a-bda7-4614-8881-f2ac618cff8e"/>
@@ -4001,22 +4016,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E254D28-D3D4-49BF-9139-FF4FDEF467DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E21D230-F0FF-46F1-8C9B-DF853E5491B6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00A2FE85-4E03-4320-929A-8E66617AF346}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4033,21 +4050,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E21D230-F0FF-46F1-8C9B-DF853E5491B6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E254D28-D3D4-49BF-9139-FF4FDEF467DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
midlands west venue update
</commit_message>
<xml_diff>
--- a/src/main/resources/venueAddressValues.xlsx
+++ b/src/main/resources/venueAddressValues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tensaybulcha/Documents/GitHub/Reformed-ET/ethos-repl-docmosis-service/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4E89AF-F186-5E4E-BAC5-F2C5BAA2E838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CDEDC8-4ACA-BD48-AD36-0937BB91BECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="56720" yWindow="500" windowWidth="30720" windowHeight="16420" activeTab="1" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
+    <workbookView xWindow="58200" yWindow="500" windowWidth="30720" windowHeight="16420" activeTab="7" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
   </bookViews>
   <sheets>
     <sheet name="Bristol" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="297">
   <si>
     <t>Leeds</t>
   </si>
@@ -1322,6 +1322,12 @@
   </si>
   <si>
     <t>2nd Floor, West Gate , 6 Grace Street, Leeds, LS1 2RP</t>
+  </si>
+  <si>
+    <t>North Staffordshire Justice Centre</t>
+  </si>
+  <si>
+    <t>The Court House, Ryecroft, Newcastle-under-Lyme, ST5 2AA</t>
   </si>
 </sst>
 </file>
@@ -3003,7 +3009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5FBCDA9-DEB7-ED42-9C1E-52C20E93783E}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -3569,15 +3575,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F0AF1F5-7AB7-9E48-BD29-64A04867FE46}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="37" style="1" customWidth="1"/>
     <col min="2" max="2" width="114.1640625" style="1" customWidth="1"/>
     <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -3640,25 +3646,33 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>92</v>
+        <v>295</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>92</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>218</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>219</v>
       </c>
     </row>
@@ -3790,6 +3804,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E98ADB2028FC4F43824F86666CC83903" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ff47f26d8558bca2ac2c896a7e751c25">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bc19a69a-bda7-4614-8881-f2ac618cff8e" xmlns:ns4="02128cc3-8226-4d54-9246-100bb62c9520" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="63ef4ea587d9ab0193671c85d2373b1f" ns3:_="" ns4:_="">
     <xsd:import namespace="bc19a69a-bda7-4614-8881-f2ac618cff8e"/>
@@ -4006,15 +4029,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E254D28-D3D4-49BF-9139-FF4FDEF467DC}">
   <ds:schemaRefs>
@@ -4025,6 +4039,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E21D230-F0FF-46F1-8C9B-DF853E5491B6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00A2FE85-4E03-4320-929A-8E66617AF346}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4041,12 +4063,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E21D230-F0FF-46F1-8C9B-DF853E5491B6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added LondonCentral address (#2647)
</commit_message>
<xml_diff>
--- a/src/main/resources/venueAddressValues.xlsx
+++ b/src/main/resources/venueAddressValues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tensaybulcha/Documents/GitHub/Reformed-ET/ethos-repl-docmosis-service/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harpreet.jhita/IdeaProjects/ethos-repl-docmosis-service/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CDEDC8-4ACA-BD48-AD36-0937BB91BECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8895929D-1EEF-D449-A4E8-C561DECEA9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58200" yWindow="500" windowWidth="30720" windowHeight="16420" activeTab="7" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="68800" windowHeight="28300" activeTab="2" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
   </bookViews>
   <sheets>
     <sheet name="Bristol" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="299">
   <si>
     <t>Leeds</t>
   </si>
@@ -1328,6 +1328,12 @@
   </si>
   <si>
     <t>The Court House, Ryecroft, Newcastle-under-Lyme, ST5 2AA</t>
+  </si>
+  <si>
+    <t>London Tribunals Centre</t>
+  </si>
+  <si>
+    <t>7 Newgate Street, London, EC1A 7AZ</t>
   </si>
 </sst>
 </file>
@@ -3107,10 +3113,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A83124E0-110E-9845-8B86-53627F72C6F1}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -3154,9 +3160,17 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>52</v>
       </c>
     </row>
@@ -3577,7 +3591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F0AF1F5-7AB7-9E48-BD29-64A04867FE46}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -3798,21 +3812,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E98ADB2028FC4F43824F86666CC83903" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ff47f26d8558bca2ac2c896a7e751c25">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bc19a69a-bda7-4614-8881-f2ac618cff8e" xmlns:ns4="02128cc3-8226-4d54-9246-100bb62c9520" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="63ef4ea587d9ab0193671c85d2373b1f" ns3:_="" ns4:_="">
     <xsd:import namespace="bc19a69a-bda7-4614-8881-f2ac618cff8e"/>
@@ -4029,24 +4028,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E254D28-D3D4-49BF-9139-FF4FDEF467DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E21D230-F0FF-46F1-8C9B-DF853E5491B6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00A2FE85-4E03-4320-929A-8E66617AF346}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4063,4 +4060,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E21D230-F0FF-46F1-8C9B-DF853E5491B6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E254D28-D3D4-49BF-9139-FF4FDEF467DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added new venue GTC to venueAddressValues.xlsx for scotland.
</commit_message>
<xml_diff>
--- a/src/main/resources/venueAddressValues.xlsx
+++ b/src/main/resources/venueAddressValues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harpreet.jhita/IdeaProjects/ethos-repl-docmosis-service/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mehmet.dede/dev/IntelliJ/ecm/ethos-repl-docmosis-service/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8895929D-1EEF-D449-A4E8-C561DECEA9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A321A780-45E8-2742-837C-D31FFF3AC2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="68800" windowHeight="28300" activeTab="2" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19680" activeTab="9" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
   </bookViews>
   <sheets>
     <sheet name="Bristol" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="300">
   <si>
     <t>Leeds</t>
   </si>
@@ -1334,6 +1334,9 @@
   </si>
   <si>
     <t>7 Newgate Street, London, EC1A 7AZ</t>
+  </si>
+  <si>
+    <t>GTC</t>
   </si>
 </sst>
 </file>
@@ -2105,10 +2108,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DABB460-37E4-BC4E-8C69-80DBA2CDCD9B}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2304,6 +2307,14 @@
       </c>
       <c r="B24" s="1" t="s">
         <v>266</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -3115,7 +3126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A83124E0-110E-9845-8B86-53627F72C6F1}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -4029,18 +4040,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4063,18 +4074,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E21D230-F0FF-46F1-8C9B-DF853E5491B6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E254D28-D3D4-49BF-9139-FF4FDEF467DC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E21D230-F0FF-46F1-8C9B-DF853E5491B6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added new venues GTC, OET Scotland, Aberdeen to venueAddressValues.xlsx for scotland. Removed one empty line that was after Tribunal venue name.
</commit_message>
<xml_diff>
--- a/src/main/resources/venueAddressValues.xlsx
+++ b/src/main/resources/venueAddressValues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mehmet.dede/dev/IntelliJ/ecm/ethos-repl-docmosis-service/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A321A780-45E8-2742-837C-D31FFF3AC2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB1B732-6210-7E41-95E7-43B5107F1554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19680" activeTab="9" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="9" xr2:uid="{57ECFE3E-99BE-FC40-B6CA-F6152164B97B}"/>
   </bookViews>
   <sheets>
     <sheet name="Bristol" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="302">
   <si>
     <t>Leeds</t>
   </si>
@@ -831,9 +831,6 @@
   </si>
   <si>
     <t>Longman Road, Inverness, IV1 1AH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tribunal </t>
   </si>
   <si>
     <t>Ground Floor, Endeavour House, 1 Greenmarket, Dundee, DD1 4QB</t>
@@ -1337,6 +1334,15 @@
   </si>
   <si>
     <t>GTC</t>
+  </si>
+  <si>
+    <t>OET Scotland</t>
+  </si>
+  <si>
+    <t>OET 54-56 Melville Street, Edinburgh, EH3 7HF</t>
+  </si>
+  <si>
+    <t>Tribunal</t>
   </si>
 </sst>
 </file>
@@ -2108,10 +2114,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DABB460-37E4-BC4E-8C69-80DBA2CDCD9B}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2303,18 +2309,34 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>191</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -2353,7 +2375,7 @@
         <v>104</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2369,7 +2391,7 @@
         <v>106</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2401,7 +2423,7 @@
         <v>110</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2417,7 +2439,7 @@
         <v>112</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2425,7 +2447,7 @@
         <v>113</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2449,7 +2471,7 @@
         <v>116</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2481,7 +2503,7 @@
         <v>120</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2569,7 +2591,7 @@
         <v>131</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2625,7 +2647,7 @@
         <v>138</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2641,7 +2663,7 @@
         <v>140</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -2673,7 +2695,7 @@
         <v>144</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2713,7 +2735,7 @@
         <v>149</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -2729,7 +2751,7 @@
         <v>151</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2737,7 +2759,7 @@
         <v>152</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2745,7 +2767,7 @@
         <v>153</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2785,7 +2807,7 @@
         <v>158</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -2801,7 +2823,7 @@
         <v>160</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -2833,7 +2855,7 @@
         <v>164</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -2841,7 +2863,7 @@
         <v>165</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -2857,7 +2879,7 @@
         <v>167</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -2873,7 +2895,7 @@
         <v>262</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -3006,7 +3028,7 @@
         <v>177</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -3071,10 +3093,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3114,7 +3136,7 @@
         <v>261</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -3171,10 +3193,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>297</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3550,7 +3572,7 @@
         <v>81</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -3671,10 +3693,10 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3811,10 +3833,10 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -3823,6 +3845,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E98ADB2028FC4F43824F86666CC83903" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ff47f26d8558bca2ac2c896a7e751c25">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bc19a69a-bda7-4614-8881-f2ac618cff8e" xmlns:ns4="02128cc3-8226-4d54-9246-100bb62c9520" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="63ef4ea587d9ab0193671c85d2373b1f" ns3:_="" ns4:_="">
     <xsd:import namespace="bc19a69a-bda7-4614-8881-f2ac618cff8e"/>
@@ -4039,12 +4067,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4055,6 +4077,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E254D28-D3D4-49BF-9139-FF4FDEF467DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00A2FE85-4E03-4320-929A-8E66617AF346}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4073,15 +4104,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E254D28-D3D4-49BF-9139-FF4FDEF467DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E21D230-F0FF-46F1-8C9B-DF853E5491B6}">
   <ds:schemaRefs>

</xml_diff>